<commit_message>
cap nhat file database
</commit_message>
<xml_diff>
--- a/2023/ViMo.xlsx
+++ b/2023/ViMo.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trung.nguyenhoang/Documents/github/2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trung.nguyenhoang/Desktop/stocks/2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70B6783-2378-614C-8504-A6473CC7349B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF4DDD0-C153-2B4F-BCC1-C058C23A275D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17080" xr2:uid="{8AA0C1B0-8D13-1E4D-8E67-BD831CFDFC4F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16940" xr2:uid="{8AA0C1B0-8D13-1E4D-8E67-BD831CFDFC4F}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>LÃI SUẤT</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>Vạn Thịnh Phát</t>
+  </si>
+  <si>
+    <t>Bất ổn ở khu vực Biển Đỏ</t>
   </si>
 </sst>
 </file>
@@ -281,82 +284,70 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -675,7 +666,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -695,257 +686,259 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="2"/>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="76" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="14" t="s">
+      <c r="E2" s="1"/>
+      <c r="F2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="14" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="12" t="s">
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="73" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="11" t="s">
+      <c r="E3" s="14"/>
+      <c r="F3" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="5" t="s">
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="7"/>
-      <c r="N3" s="5" t="s">
+      <c r="M3" s="14"/>
+      <c r="N3" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="7"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="13"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="6"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="16"/>
     </row>
     <row r="5" spans="1:14" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="7"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="14"/>
       <c r="H5" s="13"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="6"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="16"/>
     </row>
     <row r="6" spans="1:14" ht="80" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="14" t="s">
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="8" t="s">
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="M6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="N6" s="2"/>
+      <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="8" t="s">
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="14" t="s">
+      <c r="M7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="N7" s="2"/>
+      <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="19" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="8" t="s">
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="14" t="s">
+      <c r="M8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="N8" s="2"/>
+      <c r="N8" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="E3:E5"/>
     <mergeCell ref="H3:H5"/>
     <mergeCell ref="I3:I5"/>
     <mergeCell ref="J3:J5"/>
     <mergeCell ref="M3:M5"/>
     <mergeCell ref="K3:K5"/>
     <mergeCell ref="L3:L5"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="N3:N5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>